<commit_message>
data collection in excel
</commit_message>
<xml_diff>
--- a/NFES_Review/_AllData.xlsx
+++ b/NFES_Review/_AllData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oskat\OneDrive - Instituto Tecnologico y de Estudios Superiores de Monterrey\Documents\MNT_ITESM_Thesis\NFES_Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068ACC6E-2445-454F-9045-B254824578A0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0841FD-353C-4E0A-8DBB-7F97106DD985}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20220" yWindow="2760" windowWidth="16335" windowHeight="11385" xr2:uid="{257EF4C4-23DC-41CA-B233-C9469FC7ABC0}"/>
+    <workbookView xWindow="12465" yWindow="2760" windowWidth="16335" windowHeight="11385" xr2:uid="{257EF4C4-23DC-41CA-B233-C9469FC7ABC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="83">
   <si>
     <t>ref</t>
   </si>
@@ -69,9 +69,6 @@
     <t>LV NFES</t>
   </si>
   <si>
-    <t>27 gauge</t>
-  </si>
-  <si>
     <t>deposition rate [uL/h]</t>
   </si>
   <si>
@@ -114,13 +111,178 @@
     <t>typical</t>
   </si>
   <si>
-    <t>26 gauge</t>
-  </si>
-  <si>
-    <t>nozzleSubDist [um]</t>
-  </si>
-  <si>
     <t>SiO2</t>
+  </si>
+  <si>
+    <t>Chang 2008</t>
+  </si>
+  <si>
+    <t>Scanning Tip</t>
+  </si>
+  <si>
+    <t>Duang 2017</t>
+  </si>
+  <si>
+    <t>PVDF</t>
+  </si>
+  <si>
+    <t>DMF</t>
+  </si>
+  <si>
+    <t>Helix EHD</t>
+  </si>
+  <si>
+    <t>nozzleSubDist [mm]</t>
+  </si>
+  <si>
+    <t>PDMS</t>
+  </si>
+  <si>
+    <t>Gupta 2007</t>
+  </si>
+  <si>
+    <t>POSS-PCU</t>
+  </si>
+  <si>
+    <t>POSS-PCL-PCU</t>
+  </si>
+  <si>
+    <t>DMAC</t>
+  </si>
+  <si>
+    <t>Butanol</t>
+  </si>
+  <si>
+    <t>EHD jetting</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>MES</t>
+  </si>
+  <si>
+    <t>Huang 2015</t>
+  </si>
+  <si>
+    <t>Ethanol</t>
+  </si>
+  <si>
+    <t>Blow EDW</t>
+  </si>
+  <si>
+    <t>Jiang 2018</t>
+  </si>
+  <si>
+    <t>Acetone</t>
+  </si>
+  <si>
+    <t>DMSO</t>
+  </si>
+  <si>
+    <t>3D ES</t>
+  </si>
+  <si>
+    <t>paper</t>
+  </si>
+  <si>
+    <t>Kim 2018</t>
+  </si>
+  <si>
+    <t>PVK</t>
+  </si>
+  <si>
+    <t>Styrene</t>
+  </si>
+  <si>
+    <t>NFES</t>
+  </si>
+  <si>
+    <t>Min 2013</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>TCB</t>
+  </si>
+  <si>
+    <t>Song 2015</t>
+  </si>
+  <si>
+    <t>Sun 2006</t>
+  </si>
+  <si>
+    <t>MultiNozz</t>
+  </si>
+  <si>
+    <t>Wang 2015</t>
+  </si>
+  <si>
+    <t>Wang 2017</t>
+  </si>
+  <si>
+    <t>Cr</t>
+  </si>
+  <si>
+    <t>Wang 2018</t>
+  </si>
+  <si>
+    <t>Xu 2014</t>
+  </si>
+  <si>
+    <t>Gelatin</t>
+  </si>
+  <si>
+    <t>Acetic Acid</t>
+  </si>
+  <si>
+    <t>Ethyl Acetate</t>
+  </si>
+  <si>
+    <t>Xue 2014</t>
+  </si>
+  <si>
+    <t>Zheng 2010</t>
+  </si>
+  <si>
+    <t>EDW</t>
+  </si>
+  <si>
+    <t>PET</t>
+  </si>
+  <si>
+    <t>Zheng 2014</t>
+  </si>
+  <si>
+    <t>PLGA</t>
+  </si>
+  <si>
+    <t>DMC</t>
+  </si>
+  <si>
+    <t>TPES</t>
+  </si>
+  <si>
+    <t>PTFE</t>
+  </si>
+  <si>
+    <t>Coppola 2014</t>
+  </si>
+  <si>
+    <t>Brass</t>
+  </si>
+  <si>
+    <t>Cisquella-Serra 2019</t>
+  </si>
+  <si>
+    <t>Suspension</t>
+  </si>
+  <si>
+    <t>Nagle 2019</t>
+  </si>
+  <si>
+    <t>Shin 2018</t>
   </si>
 </sst>
 </file>
@@ -251,7 +413,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1E4218DC-FC6D-4499-9BCF-D3E4DA398E43}" type="CELLRANGE">
+                    <a:fld id="{FC09D92A-2BDD-42FF-8C8A-D849E6BB23E0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -336,15 +498,16 @@
             </c:extLst>
           </c:dLbls>
           <c:xVal>
-            <c:strRef>
+            <c:numRef>
               <c:f>Sheet1!$G$2</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>27 gauge</c:v>
+                  <c:v>210</c:v>
                 </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
@@ -426,7 +589,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CEB9F625-CF8C-4064-B51C-5DC412C29680}" type="CELLRANGE">
+                    <a:fld id="{9047EBAC-7D0C-4321-8574-065072E5B30B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -464,7 +627,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{48027D01-5FF6-469F-BBB4-53D013C46A65}" type="CELLRANGE">
+                    <a:fld id="{2EA666CF-A0B3-4722-923E-A292E013D0EB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -502,7 +665,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{35EA9BD1-C1A3-4A5D-BCCB-9ED02D8092ED}" type="CELLRANGE">
+                    <a:fld id="{64307F63-1D59-4864-BF3F-33557671D7D6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -540,7 +703,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7C191C12-7CE6-4FBD-92E9-AF8946F5B7D1}" type="CELLRANGE">
+                    <a:fld id="{317B4E7B-F87F-4877-9DD6-063012F6B87A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -578,7 +741,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{14375FD2-9B2B-4674-822A-2C504A85CE8A}" type="CELLRANGE">
+                    <a:fld id="{F7B634B6-60B5-4514-8651-478D7F1CA087}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -616,7 +779,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{90468128-1CFE-418A-B906-F972CD2500BD}" type="CELLRANGE">
+                    <a:fld id="{B1725766-728F-49F6-8023-D88011F78C2F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -654,7 +817,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3204C1A4-D596-43A0-A3E6-410817292947}" type="CELLRANGE">
+                    <a:fld id="{B5B7C277-8071-4A7F-A0D5-034C415E905C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -692,7 +855,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7E828FAA-DC2A-46FB-9C6D-5F3F6CFA9E35}" type="CELLRANGE">
+                    <a:fld id="{0E97F99A-6768-41A6-B5B8-77F2B2A732A8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -724,7 +887,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3AAF2DD8-C718-4361-AAB0-089037B190A6}" type="CELLRANGE">
+                    <a:fld id="{6B60BE50-4990-414B-9DFA-AD8DBCC7791C}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -763,7 +926,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D6DA7956-6250-481F-82D2-DE9198FFBECD}" type="CELLRANGE">
+                    <a:fld id="{4B92A796-1412-4E81-82DE-315E472CC6EB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -801,7 +964,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9BD39F8B-D056-43BF-9A74-FF392E707D9B}" type="CELLRANGE">
+                    <a:fld id="{52635658-E2C1-445C-85E3-6BCAE423E164}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -839,7 +1002,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FA6D004E-ABC8-4CF3-8486-FAA94476D3B6}" type="CELLRANGE">
+                    <a:fld id="{FF727329-D541-4135-A1EF-E31FF25CC25F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -877,7 +1040,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{17FEA3EB-422B-4D43-8EF9-B2DA2E64127E}" type="CELLRANGE">
+                    <a:fld id="{E0EF4873-39CD-4AC4-AE7A-917B6DACE35D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -915,7 +1078,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C15EC7B4-BA8A-46FC-BA1E-40CCCAADA7EB}" type="CELLRANGE">
+                    <a:fld id="{80003F45-87AC-4272-97F6-6D8087742639}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -953,7 +1116,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FF268658-6AF4-43AE-A53B-76BC6A560933}" type="CELLRANGE">
+                    <a:fld id="{895E5F7D-6A31-4216-A407-D72845B76804}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -991,7 +1154,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{993CD24D-8B2B-4807-96CA-B7178343257D}" type="CELLRANGE">
+                    <a:fld id="{6BCDBF85-DC45-44AA-A383-6CAD46512640}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1079,33 +1242,54 @@
             <c:strRef>
               <c:f>Sheet1!$G$3:$G$18</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>27 gauge</c:v>
+                  <c:v>210</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27 gauge</c:v>
+                  <c:v>210</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27 gauge</c:v>
+                  <c:v>210</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27 gauge</c:v>
+                  <c:v>210</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27 gauge</c:v>
+                  <c:v>210</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26 gauge</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26 gauge</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26 gauge</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>26 gauge</c:v>
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>NA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1142,6 +1326,27 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1180,6 +1385,27 @@
                   <c:pt idx="8">
                     <c:v>PEO</c:v>
                   </c:pt>
+                  <c:pt idx="9">
+                    <c:v>PEO</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>PVDF</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>POSS-PCU</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>POSS-PCL-PCU</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>POSS-PCU</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>POSS-PCL-PCU</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>PEO</c:v>
+                  </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
             </c:ext>
@@ -1196,6 +1422,9 @@
               <c:f>Sheet1!$D$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Water</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -1251,7 +1480,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F8A62756-AC5B-4BA7-9709-4ABDE8B8980C}" type="CELLRANGE">
+                    <a:fld id="{8267306F-4BA1-4EB3-9954-949E9A293852}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1343,6 +1572,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>210</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1352,6 +1584,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1362,6 +1597,9 @@
                 <c15:f>Sheet1!$B$19</c15:f>
                 <c15:dlblRangeCache>
                   <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>PEO</c:v>
+                  </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
             </c:ext>
@@ -1378,6 +1616,9 @@
               <c:f>Sheet1!$D$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Acetone</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -1417,7 +1658,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B4E9709C-D682-4B9A-8F51-D52FD9579AA7}" type="CELLRANGE">
+                    <a:fld id="{AA277152-4DB0-48D4-B0FC-749DF12CAA60}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1455,7 +1696,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{64CECCC0-DFD1-47AA-8698-3CF75417BA26}" type="CELLRANGE">
+                    <a:fld id="{9FE2B48A-CAB9-401E-B6D5-C2EE4F3F6717}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1545,6 +1786,12 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1554,6 +1801,12 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1564,6 +1817,12 @@
                 <c15:f>Sheet1!$B$21:$B$22</c15:f>
                 <c15:dlblRangeCache>
                   <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>PVDF</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>PVDF</c:v>
+                  </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
             </c:ext>
@@ -1580,6 +1839,9 @@
               <c:f>Sheet1!$D$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Styrene</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -1613,7 +1875,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2307F092-1B1B-4136-BC91-02114D8E678C}" type="CELLRANGE">
+                    <a:fld id="{5582D749-2A63-4064-A2F9-15E67683E999}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1703,6 +1965,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1712,6 +1977,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3.96</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1722,6 +1990,9 @@
                 <c15:f>Sheet1!$B$23</c15:f>
                 <c15:dlblRangeCache>
                   <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>PVK</c:v>
+                  </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
             </c:ext>
@@ -2961,27 +3232,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33050BF9-30EE-4B25-89E8-D0C2AB98776D}">
-  <dimension ref="A1:O55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33050BF9-30EE-4B25-89E8-D0C2AB98776D}">
+  <dimension ref="A1:O43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="9" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -2990,31 +3276,31 @@
         <v>7</v>
       </c>
       <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
-        <v>18</v>
-      </c>
       <c r="H1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="J1" t="s">
         <v>8</v>
       </c>
       <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>20</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>21</v>
-      </c>
-      <c r="N1" t="s">
-        <v>22</v>
       </c>
       <c r="O1" t="s">
         <v>0</v>
@@ -3039,17 +3325,17 @@
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
-        <v>11</v>
+      <c r="G2">
+        <v>210</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K2">
         <v>300</v>
@@ -3061,7 +3347,7 @@
         <v>237</v>
       </c>
       <c r="N2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O2" t="s">
         <v>3</v>
@@ -3086,17 +3372,17 @@
       <c r="F3">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
-        <v>11</v>
+      <c r="G3">
+        <v>210</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K3">
         <v>300</v>
@@ -3108,7 +3394,7 @@
         <v>237</v>
       </c>
       <c r="N3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O3" t="s">
         <v>3</v>
@@ -3133,17 +3419,17 @@
       <c r="F4">
         <v>3</v>
       </c>
-      <c r="G4" t="s">
-        <v>11</v>
+      <c r="G4">
+        <v>210</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="I4">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K4">
         <v>300</v>
@@ -3155,7 +3441,7 @@
         <v>237</v>
       </c>
       <c r="N4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O4" t="s">
         <v>3</v>
@@ -3180,17 +3466,17 @@
       <c r="F5">
         <v>1</v>
       </c>
-      <c r="G5" t="s">
-        <v>11</v>
+      <c r="G5">
+        <v>210</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
       <c r="I5">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K5">
         <v>300</v>
@@ -3202,7 +3488,7 @@
         <v>237</v>
       </c>
       <c r="N5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O5" t="s">
         <v>3</v>
@@ -3227,17 +3513,17 @@
       <c r="F6">
         <v>2</v>
       </c>
-      <c r="G6" t="s">
-        <v>11</v>
+      <c r="G6">
+        <v>210</v>
       </c>
       <c r="H6">
         <v>1</v>
       </c>
       <c r="I6">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K6">
         <v>300</v>
@@ -3249,7 +3535,7 @@
         <v>237</v>
       </c>
       <c r="N6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O6" t="s">
         <v>3</v>
@@ -3274,17 +3560,17 @@
       <c r="F7">
         <v>3</v>
       </c>
-      <c r="G7" t="s">
-        <v>11</v>
+      <c r="G7">
+        <v>210</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
       <c r="I7">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K7">
         <v>300</v>
@@ -3296,7 +3582,7 @@
         <v>237</v>
       </c>
       <c r="N7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O7" t="s">
         <v>3</v>
@@ -3313,25 +3599,25 @@
         <v>380000</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F8">
         <v>0.08</v>
       </c>
-      <c r="G8" t="s">
-        <v>26</v>
+      <c r="G8">
+        <v>260</v>
       </c>
       <c r="H8">
         <v>50</v>
       </c>
       <c r="I8">
-        <v>500</v>
+        <v>0.5</v>
       </c>
       <c r="J8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K8">
         <v>1300</v>
@@ -3360,25 +3646,25 @@
         <v>300000</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9">
         <v>0.08</v>
       </c>
-      <c r="G9" t="s">
-        <v>26</v>
+      <c r="G9">
+        <v>260</v>
       </c>
       <c r="H9">
         <v>50</v>
       </c>
       <c r="I9">
-        <v>500</v>
+        <v>0.5</v>
       </c>
       <c r="J9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K9">
         <v>1300</v>
@@ -3407,25 +3693,25 @@
         <v>380000</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10">
         <v>0.08</v>
       </c>
-      <c r="G10" t="s">
-        <v>26</v>
+      <c r="G10">
+        <v>260</v>
       </c>
       <c r="H10">
         <v>50</v>
       </c>
       <c r="I10">
-        <v>500</v>
+        <v>0.5</v>
       </c>
       <c r="J10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K10">
         <v>1300</v>
@@ -3454,25 +3740,25 @@
         <v>300000</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F11">
         <v>0.08</v>
       </c>
-      <c r="G11" t="s">
-        <v>26</v>
+      <c r="G11">
+        <v>260</v>
       </c>
       <c r="H11">
         <v>50</v>
       </c>
       <c r="I11">
-        <v>500</v>
+        <v>0.5</v>
       </c>
       <c r="J11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K11">
         <v>1300</v>
@@ -3494,220 +3780,1504 @@
       <c r="A12">
         <v>10</v>
       </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>300000</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12">
+        <v>7</v>
+      </c>
+      <c r="G12">
+        <v>100</v>
+      </c>
+      <c r="H12">
+        <v>0.1</v>
+      </c>
+      <c r="I12">
+        <v>0.5</v>
+      </c>
+      <c r="J12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12">
+        <v>800</v>
+      </c>
+      <c r="L12">
+        <v>120</v>
+      </c>
+      <c r="M12">
+        <v>61</v>
+      </c>
+      <c r="N12" t="s">
+        <v>14</v>
+      </c>
+      <c r="O12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13">
+        <v>440000</v>
+      </c>
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13">
+        <v>18</v>
+      </c>
+      <c r="G13">
+        <v>260</v>
+      </c>
+      <c r="H13">
+        <v>24</v>
+      </c>
+      <c r="I13">
+        <v>30</v>
+      </c>
+      <c r="J13" t="s">
+        <v>33</v>
+      </c>
+      <c r="K13">
+        <v>2250</v>
+      </c>
+      <c r="L13">
+        <v>6.6669999999999998</v>
+      </c>
+      <c r="M13">
+        <v>2250</v>
+      </c>
+      <c r="N13" t="s">
+        <v>14</v>
+      </c>
+      <c r="O13" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14">
+        <v>2000</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14">
+        <v>20</v>
+      </c>
+      <c r="G14">
+        <v>750</v>
+      </c>
+      <c r="H14">
+        <v>60</v>
+      </c>
+      <c r="I14">
+        <v>1.25</v>
+      </c>
+      <c r="J14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14">
+        <v>9000</v>
+      </c>
+      <c r="L14">
+        <v>10</v>
+      </c>
+      <c r="M14">
+        <v>27500</v>
+      </c>
+      <c r="N14">
+        <v>250</v>
+      </c>
+      <c r="O14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15">
+        <v>2000</v>
+      </c>
+      <c r="D15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15">
+        <v>20</v>
+      </c>
+      <c r="G15">
+        <v>750</v>
+      </c>
+      <c r="H15">
+        <v>60</v>
+      </c>
+      <c r="I15">
+        <v>1.25</v>
+      </c>
+      <c r="J15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15">
+        <v>9000</v>
+      </c>
+      <c r="L15">
+        <v>10</v>
+      </c>
+      <c r="M15">
+        <v>27500</v>
+      </c>
+      <c r="N15">
+        <v>250</v>
+      </c>
+      <c r="O15" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16">
+        <v>2000</v>
+      </c>
+      <c r="D16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16">
+        <v>20</v>
+      </c>
+      <c r="G16">
+        <v>750</v>
+      </c>
+      <c r="H16">
+        <v>60</v>
+      </c>
+      <c r="I16">
+        <v>1.25</v>
+      </c>
+      <c r="J16" t="s">
+        <v>14</v>
+      </c>
+      <c r="K16">
+        <v>9000</v>
+      </c>
+      <c r="L16">
+        <v>10</v>
+      </c>
+      <c r="M16">
+        <v>27500</v>
+      </c>
+      <c r="N16">
+        <v>250</v>
+      </c>
+      <c r="O16" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17">
+        <v>2000</v>
+      </c>
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17">
+        <v>20</v>
+      </c>
+      <c r="G17">
+        <v>750</v>
+      </c>
+      <c r="H17">
+        <v>60</v>
+      </c>
+      <c r="I17">
+        <v>1.25</v>
+      </c>
+      <c r="J17" t="s">
+        <v>14</v>
+      </c>
+      <c r="K17">
+        <v>9000</v>
+      </c>
+      <c r="L17">
+        <v>10</v>
+      </c>
+      <c r="M17">
+        <v>27500</v>
+      </c>
+      <c r="N17">
+        <v>250</v>
+      </c>
+      <c r="O17" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>300000</v>
+      </c>
+      <c r="D18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18">
+        <v>6</v>
+      </c>
+      <c r="G18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18">
+        <v>72000</v>
+      </c>
+      <c r="I18">
+        <v>7.5</v>
+      </c>
+      <c r="J18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K18">
+        <v>900</v>
+      </c>
+      <c r="L18">
+        <v>400</v>
+      </c>
+      <c r="M18">
+        <v>275</v>
+      </c>
+      <c r="N18">
+        <v>5</v>
+      </c>
+      <c r="O18" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>30000</v>
+      </c>
+      <c r="D19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19">
+        <v>8</v>
+      </c>
+      <c r="G19">
+        <v>210</v>
+      </c>
+      <c r="H19">
+        <v>30</v>
+      </c>
+      <c r="I19">
+        <v>2</v>
+      </c>
+      <c r="J19" t="s">
+        <v>13</v>
+      </c>
+      <c r="K19">
+        <v>2000</v>
+      </c>
+      <c r="L19">
+        <v>10.5</v>
+      </c>
+      <c r="M19">
+        <v>3730</v>
+      </c>
+      <c r="N19">
+        <v>5.13</v>
+      </c>
+      <c r="O19" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>30000</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20">
+        <v>8</v>
+      </c>
+      <c r="G20">
+        <v>210</v>
+      </c>
+      <c r="H20">
+        <v>30</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+      <c r="J20" t="s">
+        <v>13</v>
+      </c>
+      <c r="K20">
+        <v>2000</v>
+      </c>
+      <c r="L20">
+        <v>10.5</v>
+      </c>
+      <c r="M20">
+        <v>3730</v>
+      </c>
+      <c r="N20">
+        <v>5.13</v>
+      </c>
+      <c r="O20" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21">
+        <v>534000</v>
+      </c>
+      <c r="D21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21">
+        <v>17</v>
+      </c>
+      <c r="G21">
+        <v>100</v>
+      </c>
+      <c r="H21">
+        <v>0.84</v>
+      </c>
+      <c r="I21">
+        <v>0.75</v>
+      </c>
+      <c r="J21" t="s">
+        <v>49</v>
+      </c>
+      <c r="K21">
+        <v>1900</v>
+      </c>
+      <c r="L21">
+        <v>10</v>
+      </c>
+      <c r="M21" t="s">
+        <v>14</v>
+      </c>
+      <c r="N21" t="s">
+        <v>14</v>
+      </c>
+      <c r="O21" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22">
+        <v>534000</v>
+      </c>
+      <c r="D22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22">
+        <v>17</v>
+      </c>
+      <c r="G22">
+        <v>100</v>
+      </c>
+      <c r="H22">
+        <v>0.84</v>
+      </c>
+      <c r="I22">
+        <v>0.75</v>
+      </c>
+      <c r="J22" t="s">
+        <v>49</v>
+      </c>
+      <c r="K22">
+        <v>1900</v>
+      </c>
+      <c r="L22">
+        <v>10</v>
+      </c>
+      <c r="M22" t="s">
+        <v>14</v>
+      </c>
+      <c r="N22" t="s">
+        <v>14</v>
+      </c>
+      <c r="O22" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23">
+        <v>1100000</v>
+      </c>
+      <c r="D23" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23">
+        <v>3.96</v>
+      </c>
+      <c r="G23">
+        <v>100</v>
+      </c>
+      <c r="H23">
+        <v>30</v>
+      </c>
+      <c r="I23">
+        <v>2.5</v>
+      </c>
+      <c r="J23" t="s">
+        <v>13</v>
+      </c>
+      <c r="K23">
+        <v>3500</v>
+      </c>
+      <c r="L23">
+        <v>133</v>
+      </c>
+      <c r="M23">
+        <v>289.26</v>
+      </c>
+      <c r="N23">
+        <v>50</v>
+      </c>
+      <c r="O23" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24">
+        <v>1100000</v>
+      </c>
+      <c r="D24" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24">
+        <v>3.96</v>
+      </c>
+      <c r="G24">
+        <v>100</v>
+      </c>
+      <c r="H24">
+        <v>30</v>
+      </c>
+      <c r="I24">
+        <v>2.5</v>
+      </c>
+      <c r="J24" t="s">
+        <v>25</v>
+      </c>
+      <c r="K24">
+        <v>3500</v>
+      </c>
+      <c r="L24">
+        <v>133</v>
+      </c>
+      <c r="M24">
+        <v>289.26</v>
+      </c>
+      <c r="N24">
+        <v>50</v>
+      </c>
+      <c r="O24" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
+      <c r="B25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" t="s">
+        <v>39</v>
+      </c>
+      <c r="F25">
+        <v>3</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25" t="s">
+        <v>14</v>
+      </c>
+      <c r="I25">
+        <v>30</v>
+      </c>
+      <c r="J25" t="s">
+        <v>13</v>
+      </c>
+      <c r="K25">
+        <v>450</v>
+      </c>
+      <c r="L25">
+        <v>5</v>
+      </c>
+      <c r="M25">
+        <v>115000</v>
+      </c>
+      <c r="N25" t="s">
+        <v>14</v>
+      </c>
+      <c r="O25" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
+      <c r="B26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26">
+        <v>300000</v>
+      </c>
+      <c r="D26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+      <c r="G26" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" t="s">
+        <v>14</v>
+      </c>
+      <c r="I26">
+        <v>0.5</v>
+      </c>
+      <c r="J26" t="s">
+        <v>13</v>
+      </c>
+      <c r="K26">
+        <v>1000</v>
+      </c>
+      <c r="L26">
+        <v>200</v>
+      </c>
+      <c r="M26">
+        <v>30</v>
+      </c>
+      <c r="N26">
+        <v>25</v>
+      </c>
+      <c r="O26" t="s">
+        <v>58</v>
+      </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <v>2000000</v>
+      </c>
+      <c r="D27" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" t="s">
+        <v>59</v>
+      </c>
+      <c r="F27">
+        <v>5</v>
+      </c>
+      <c r="G27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27">
+        <v>120</v>
+      </c>
+      <c r="I27">
+        <v>2</v>
+      </c>
+      <c r="J27" t="s">
+        <v>14</v>
+      </c>
+      <c r="K27">
+        <v>2200</v>
+      </c>
+      <c r="L27" t="s">
+        <v>14</v>
+      </c>
+      <c r="M27">
+        <v>5470</v>
+      </c>
+      <c r="N27">
+        <v>4000</v>
+      </c>
+      <c r="O27" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
+      <c r="B28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28">
+        <v>2000000</v>
+      </c>
+      <c r="D28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" t="s">
+        <v>59</v>
+      </c>
+      <c r="F28">
+        <v>5</v>
+      </c>
+      <c r="G28">
+        <v>180</v>
+      </c>
+      <c r="H28">
+        <v>12</v>
+      </c>
+      <c r="I28">
+        <v>3.5</v>
+      </c>
+      <c r="J28" t="s">
+        <v>14</v>
+      </c>
+      <c r="K28">
+        <v>2500</v>
+      </c>
+      <c r="L28">
+        <v>20</v>
+      </c>
+      <c r="M28" t="s">
+        <v>14</v>
+      </c>
+      <c r="N28">
+        <v>272000</v>
+      </c>
+      <c r="O28" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29">
+        <v>2000000</v>
+      </c>
+      <c r="D29" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" t="s">
+        <v>59</v>
+      </c>
+      <c r="F29">
+        <v>5</v>
+      </c>
+      <c r="G29">
+        <v>180</v>
+      </c>
+      <c r="H29">
+        <v>12</v>
+      </c>
+      <c r="I29">
+        <v>4</v>
+      </c>
+      <c r="J29" t="s">
+        <v>62</v>
+      </c>
+      <c r="K29">
+        <v>2500</v>
+      </c>
+      <c r="L29">
+        <v>20</v>
+      </c>
+      <c r="M29" t="s">
+        <v>14</v>
+      </c>
+      <c r="N29">
+        <v>2511.3000000000002</v>
+      </c>
+      <c r="O29" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
+      <c r="B30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30">
+        <v>4000000</v>
+      </c>
+      <c r="D30" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F30">
+        <v>2</v>
+      </c>
+      <c r="G30">
+        <v>150</v>
+      </c>
+      <c r="H30" t="s">
+        <v>14</v>
+      </c>
+      <c r="I30">
+        <v>2</v>
+      </c>
+      <c r="J30" t="s">
+        <v>13</v>
+      </c>
+      <c r="K30">
+        <v>1250</v>
+      </c>
+      <c r="L30" t="s">
+        <v>14</v>
+      </c>
+      <c r="M30" t="s">
+        <v>14</v>
+      </c>
+      <c r="N30">
+        <v>20</v>
+      </c>
+      <c r="O30" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
+      <c r="B31" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" t="s">
+        <v>66</v>
+      </c>
+      <c r="E31" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31">
+        <v>11</v>
+      </c>
+      <c r="G31">
+        <v>1080</v>
+      </c>
+      <c r="H31" t="s">
+        <v>14</v>
+      </c>
+      <c r="I31">
+        <v>1.25</v>
+      </c>
+      <c r="J31" t="s">
+        <v>33</v>
+      </c>
+      <c r="K31">
+        <v>1000</v>
+      </c>
+      <c r="L31" t="s">
+        <v>14</v>
+      </c>
+      <c r="M31">
+        <v>2500</v>
+      </c>
+      <c r="N31">
+        <v>40</v>
+      </c>
+      <c r="O31" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
+      <c r="B32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" t="s">
+        <v>67</v>
+      </c>
+      <c r="E32" t="s">
+        <v>53</v>
+      </c>
+      <c r="F32">
+        <v>11</v>
+      </c>
+      <c r="G32">
+        <v>1080</v>
+      </c>
+      <c r="H32" t="s">
+        <v>14</v>
+      </c>
+      <c r="I32">
+        <v>1.25</v>
+      </c>
+      <c r="J32" t="s">
+        <v>33</v>
+      </c>
+      <c r="K32">
+        <v>1000</v>
+      </c>
+      <c r="L32" t="s">
+        <v>14</v>
+      </c>
+      <c r="M32">
+        <v>2500</v>
+      </c>
+      <c r="N32">
+        <v>40</v>
+      </c>
+      <c r="O32" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
+      <c r="B33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33">
+        <v>300000</v>
+      </c>
+      <c r="D33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E33" t="s">
+        <v>53</v>
+      </c>
+      <c r="F33">
+        <v>16</v>
+      </c>
+      <c r="G33">
+        <v>40</v>
+      </c>
+      <c r="H33" t="s">
+        <v>14</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33" t="s">
+        <v>13</v>
+      </c>
+      <c r="K33">
+        <v>1700</v>
+      </c>
+      <c r="L33">
+        <v>360</v>
+      </c>
+      <c r="M33">
+        <v>5150</v>
+      </c>
+      <c r="N33" t="s">
+        <v>14</v>
+      </c>
+      <c r="O33" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
+      <c r="B34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34">
+        <v>300000</v>
+      </c>
+      <c r="D34" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34">
+        <v>16</v>
+      </c>
+      <c r="G34">
+        <v>40</v>
+      </c>
+      <c r="H34" t="s">
+        <v>14</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34" t="s">
+        <v>13</v>
+      </c>
+      <c r="K34">
+        <v>1700</v>
+      </c>
+      <c r="L34">
+        <v>360</v>
+      </c>
+      <c r="M34">
+        <v>5150</v>
+      </c>
+      <c r="N34" t="s">
+        <v>14</v>
+      </c>
+      <c r="O34" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
+      <c r="B35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35">
+        <v>300000</v>
+      </c>
+      <c r="D35" t="s">
+        <v>40</v>
+      </c>
+      <c r="E35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F35">
+        <v>18</v>
+      </c>
+      <c r="G35">
+        <v>40</v>
+      </c>
+      <c r="H35" t="s">
+        <v>14</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="J35" t="s">
+        <v>13</v>
+      </c>
+      <c r="K35">
+        <v>1700</v>
+      </c>
+      <c r="L35">
+        <v>360</v>
+      </c>
+      <c r="M35">
+        <v>5150</v>
+      </c>
+      <c r="N35" t="s">
+        <v>14</v>
+      </c>
+      <c r="O35" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
+      <c r="B36" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36">
+        <v>300000</v>
+      </c>
+      <c r="D36" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" t="s">
+        <v>53</v>
+      </c>
+      <c r="F36">
+        <v>18</v>
+      </c>
+      <c r="G36">
+        <v>40</v>
+      </c>
+      <c r="H36" t="s">
+        <v>14</v>
+      </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+      <c r="J36" t="s">
+        <v>13</v>
+      </c>
+      <c r="K36">
+        <v>1700</v>
+      </c>
+      <c r="L36">
+        <v>360</v>
+      </c>
+      <c r="M36">
+        <v>5150</v>
+      </c>
+      <c r="N36" t="s">
+        <v>14</v>
+      </c>
+      <c r="O36" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37">
+        <v>300000</v>
+      </c>
+      <c r="D37" t="s">
+        <v>40</v>
+      </c>
+      <c r="E37" t="s">
+        <v>70</v>
+      </c>
+      <c r="F37">
+        <v>14</v>
+      </c>
+      <c r="G37">
+        <v>210</v>
+      </c>
+      <c r="H37">
+        <v>50</v>
+      </c>
+      <c r="I37">
+        <v>2</v>
+      </c>
+      <c r="J37" t="s">
+        <v>71</v>
+      </c>
+      <c r="K37">
+        <v>3000</v>
+      </c>
+      <c r="L37">
+        <v>700</v>
+      </c>
+      <c r="M37">
+        <v>25000</v>
+      </c>
+      <c r="N37">
+        <v>70</v>
+      </c>
+      <c r="O37" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
+      <c r="B38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38">
+        <v>300000</v>
+      </c>
+      <c r="D38" t="s">
+        <v>43</v>
+      </c>
+      <c r="E38" t="s">
+        <v>70</v>
+      </c>
+      <c r="F38">
+        <v>14</v>
+      </c>
+      <c r="G38">
+        <v>210</v>
+      </c>
+      <c r="H38">
+        <v>50</v>
+      </c>
+      <c r="I38">
+        <v>2</v>
+      </c>
+      <c r="J38" t="s">
+        <v>71</v>
+      </c>
+      <c r="K38">
+        <v>3000</v>
+      </c>
+      <c r="L38">
+        <v>700</v>
+      </c>
+      <c r="M38">
+        <v>25000</v>
+      </c>
+      <c r="N38">
+        <v>70</v>
+      </c>
+      <c r="O38" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
+      <c r="B39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" t="s">
+        <v>74</v>
+      </c>
+      <c r="E39" t="s">
+        <v>75</v>
+      </c>
+      <c r="F39" t="s">
+        <v>14</v>
+      </c>
+      <c r="G39" t="s">
+        <v>14</v>
+      </c>
+      <c r="H39" t="s">
+        <v>14</v>
+      </c>
+      <c r="I39" t="s">
+        <v>14</v>
+      </c>
+      <c r="J39" t="s">
+        <v>76</v>
+      </c>
+      <c r="K39">
+        <v>26000000</v>
+      </c>
+      <c r="L39" t="s">
+        <v>14</v>
+      </c>
+      <c r="M39">
+        <v>304.7</v>
+      </c>
+      <c r="N39" t="s">
+        <v>14</v>
+      </c>
+      <c r="O39" t="s">
+        <v>77</v>
+      </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
+      <c r="B40" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40">
+        <v>4000000</v>
+      </c>
+      <c r="D40" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40" t="s">
+        <v>53</v>
+      </c>
+      <c r="F40">
+        <v>0.75</v>
+      </c>
+      <c r="G40" t="s">
+        <v>14</v>
+      </c>
+      <c r="H40" t="s">
+        <v>14</v>
+      </c>
+      <c r="I40" t="s">
+        <v>14</v>
+      </c>
+      <c r="J40" t="s">
+        <v>78</v>
+      </c>
+      <c r="K40">
+        <v>980</v>
+      </c>
+      <c r="L40" t="s">
+        <v>14</v>
+      </c>
+      <c r="M40" t="s">
+        <v>14</v>
+      </c>
+      <c r="N40" t="s">
+        <v>14</v>
+      </c>
+      <c r="O40" t="s">
+        <v>79</v>
+      </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
+      <c r="B41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41">
+        <v>200000</v>
+      </c>
+      <c r="D41" t="s">
+        <v>40</v>
+      </c>
+      <c r="E41" t="s">
+        <v>80</v>
+      </c>
+      <c r="F41">
+        <v>14</v>
+      </c>
+      <c r="G41">
+        <v>250</v>
+      </c>
+      <c r="H41">
+        <v>10.8</v>
+      </c>
+      <c r="I41">
+        <v>5.25</v>
+      </c>
+      <c r="J41" t="s">
+        <v>13</v>
+      </c>
+      <c r="K41">
+        <v>1600</v>
+      </c>
+      <c r="L41">
+        <v>150</v>
+      </c>
+      <c r="M41">
+        <v>300</v>
+      </c>
+      <c r="N41">
+        <v>300</v>
+      </c>
+      <c r="O41" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
+      <c r="B42" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42">
+        <v>200000</v>
+      </c>
+      <c r="D42" t="s">
+        <v>43</v>
+      </c>
+      <c r="E42" t="s">
+        <v>80</v>
+      </c>
+      <c r="F42">
+        <v>14</v>
+      </c>
+      <c r="G42">
+        <v>250</v>
+      </c>
+      <c r="H42">
+        <v>10.8</v>
+      </c>
+      <c r="I42">
+        <v>5.25</v>
+      </c>
+      <c r="J42" t="s">
+        <v>13</v>
+      </c>
+      <c r="K42">
+        <v>1600</v>
+      </c>
+      <c r="L42">
+        <v>150</v>
+      </c>
+      <c r="M42">
+        <v>300</v>
+      </c>
+      <c r="N42">
+        <v>300</v>
+      </c>
+      <c r="O42" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52">
+      <c r="B43" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43">
+        <v>400000</v>
+      </c>
+      <c r="D43" t="s">
+        <v>40</v>
+      </c>
+      <c r="E43" t="s">
+        <v>53</v>
+      </c>
+      <c r="F43">
+        <v>10</v>
+      </c>
+      <c r="G43">
+        <v>108</v>
+      </c>
+      <c r="H43" t="s">
+        <v>14</v>
+      </c>
+      <c r="I43">
+        <v>0.5</v>
+      </c>
+      <c r="J43" t="s">
+        <v>13</v>
+      </c>
+      <c r="K43">
+        <v>400</v>
+      </c>
+      <c r="L43">
+        <v>5</v>
+      </c>
+      <c r="M43" t="s">
+        <v>14</v>
+      </c>
+      <c r="N43">
         <v>50</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>53</v>
+      <c r="O43" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -3715,5 +5285,6 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
nano tec presentation plus review paper progress
</commit_message>
<xml_diff>
--- a/NFES_Review/_AllData.xlsx
+++ b/NFES_Review/_AllData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oskat\OneDrive - Instituto Tecnologico y de Estudios Superiores de Monterrey\Documents\MNT_ITESM_Thesis\NFES_Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D6A942-E37E-4BC3-A12B-255FAA073905}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CCDA87E-5754-4562-9B70-27DB0E9FFB9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9675" yWindow="2310" windowWidth="16335" windowHeight="11385" activeTab="1" xr2:uid="{257EF4C4-23DC-41CA-B233-C9469FC7ABC0}"/>
+    <workbookView xWindow="345" yWindow="1950" windowWidth="22200" windowHeight="12255" activeTab="1" xr2:uid="{257EF4C4-23DC-41CA-B233-C9469FC7ABC0}"/>
   </bookViews>
   <sheets>
     <sheet name="allData" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="127">
   <si>
     <t>ref</t>
   </si>
@@ -383,6 +383,45 @@
   </si>
   <si>
     <t>1-Methyl-2-Pyrolidinone</t>
+  </si>
+  <si>
+    <t>516 Pa</t>
+  </si>
+  <si>
+    <t>vapour pressure</t>
+  </si>
+  <si>
+    <t>200 mmHg</t>
+  </si>
+  <si>
+    <t>115 mmHg</t>
+  </si>
+  <si>
+    <t>24 kPa</t>
+  </si>
+  <si>
+    <t>760 mmHg</t>
+  </si>
+  <si>
+    <t>13.02 kPa</t>
+  </si>
+  <si>
+    <t>202 kPa</t>
+  </si>
+  <si>
+    <t>4.6 kPa</t>
+  </si>
+  <si>
+    <t>53.3 kPa</t>
+  </si>
+  <si>
+    <t>5.95 kPa</t>
+  </si>
+  <si>
+    <t>96.2 mmHg</t>
+  </si>
+  <si>
+    <t>0.42 mmHg</t>
   </si>
 </sst>
 </file>
@@ -436,11 +475,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,7 +570,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8D17E2C9-2EE4-4CD4-8728-566F48F9405B}" type="CELLRANGE">
+                    <a:fld id="{DAD38BBD-581A-40F1-948F-21DD502D761A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -704,7 +746,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CA4610F1-7F4A-4825-B15C-E271966F6F0F}" type="CELLRANGE">
+                    <a:fld id="{B497DE2E-FBDC-4906-B5D1-B30104DB90A7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -742,7 +784,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{830A6278-0CC9-4568-B6B4-F41E207A5910}" type="CELLRANGE">
+                    <a:fld id="{5279F7B3-1400-4916-AC3C-F853E94458BB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -780,7 +822,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E84A62A3-FF6D-411E-A185-A472E110BDE8}" type="CELLRANGE">
+                    <a:fld id="{C2A212BE-FFE2-4E2A-822E-BC1BD6270902}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -818,7 +860,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{29510F70-93BB-4326-8D4C-364F078DE990}" type="CELLRANGE">
+                    <a:fld id="{A9AC9215-B348-42EF-9A61-05DD2D67170B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -856,7 +898,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{92953B57-09F7-4CE8-889E-D6CB47BD223C}" type="CELLRANGE">
+                    <a:fld id="{AA044EBD-7D46-4C79-9D14-2DA55BAA2AD3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -894,7 +936,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9D2F2C1E-9A7F-4587-886E-4F220744CCB3}" type="CELLRANGE">
+                    <a:fld id="{C4252435-E223-424F-AD74-C2BD61157402}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -932,7 +974,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{37154749-4B5E-4A07-93B7-BC6B74D6C202}" type="CELLRANGE">
+                    <a:fld id="{4A8A41BA-C29E-46FD-8D61-6E5233174716}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -970,7 +1012,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{24F59E8C-A503-4EC7-8FCB-6545929FA83C}" type="CELLRANGE">
+                    <a:fld id="{822F0938-7AB7-4D3D-946A-A4A8966ECAB1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1002,7 +1044,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{555E0DF0-C128-4A5B-A70C-C3EBC6FF0567}" type="CELLRANGE">
+                    <a:fld id="{7E77CA1B-C0ED-468F-B575-2EC6E2EFEA6D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1041,7 +1083,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{81F4A241-960F-4806-BE9F-6F171370E358}" type="CELLRANGE">
+                    <a:fld id="{41E3B0FB-24D1-4803-95F0-5CBEFF4C66B4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1079,7 +1121,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D184CFEF-17D5-4B2D-8FEC-B297CA7A4F33}" type="CELLRANGE">
+                    <a:fld id="{6F9EC7DC-99FA-4E0B-8560-0563B0E51FF2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1117,7 +1159,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FD8D5CFD-F5CE-422B-AB33-14385907B48C}" type="CELLRANGE">
+                    <a:fld id="{01168330-204D-4CAF-9790-36FF13ADB77C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1155,7 +1197,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{99D974AD-A217-4B08-A5C9-381B2F4B254A}" type="CELLRANGE">
+                    <a:fld id="{C1F471B6-44B2-4C4B-8258-4B1D74A06211}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1193,7 +1235,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B2A61A7F-BFA8-47B1-B3B7-CDB69F4ACCC7}" type="CELLRANGE">
+                    <a:fld id="{0EC2DE89-871E-4289-94A4-5E5278551A61}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1231,7 +1273,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6A82B363-B715-4A00-A323-8B8D1957255F}" type="CELLRANGE">
+                    <a:fld id="{A406B454-BA28-43A6-805E-0DF4F18F2555}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1269,7 +1311,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0B5C518E-2F1F-4406-A458-9ECE55B071EB}" type="CELLRANGE">
+                    <a:fld id="{57C3418E-4D56-4070-942D-35E03E5239BC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1596,7 +1638,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9E90AFCA-EFE8-46B3-8C82-23C564652F5C}" type="CELLRANGE">
+                    <a:fld id="{93254F50-68B2-4D89-88C2-C432986DB92C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1774,7 +1816,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A67A6310-A70D-47E4-8198-3DCF98936107}" type="CELLRANGE">
+                    <a:fld id="{76BF417A-C11C-418A-980E-D0EDF87A49C4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1812,7 +1854,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{762535EE-D430-4C4F-9FF3-1C180F10A812}" type="CELLRANGE">
+                    <a:fld id="{0B86031E-EB9F-4F26-8463-F6567DE60D75}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1991,7 +2033,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E9DE1408-DD59-45EB-B195-D71715358F7F}" type="CELLRANGE">
+                    <a:fld id="{791C4DDA-8E8D-48C1-B8C7-B049BF04E370}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2519,7 +2561,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{73F636B1-C9A7-47A5-9C60-8634C8E38021}" type="CELLRANGE">
+                    <a:fld id="{657EF1F3-74BB-4A5B-8A69-2E61D302EB93}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2764,7 +2806,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{10ABFBD6-5A3E-4C69-B72B-24F95C25E729}" type="CELLRANGE">
+                    <a:fld id="{C6BB8A30-3FB4-4D11-B464-783DF762387E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2803,7 +2845,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AD2AD403-79D3-4CAA-BA40-EB5F6364046E}" type="CELLRANGE">
+                    <a:fld id="{D7DE54D4-AA35-4F79-ACD4-15B21B7FF436}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2842,7 +2884,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7A9E858C-4857-4339-A362-6C3E883FC53E}" type="CELLRANGE">
+                    <a:fld id="{C16292DD-E59D-48AD-A716-2C38E372A3B3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2881,7 +2923,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ECAEF1D6-AFA1-4200-A0DB-CE549AAA36C3}" type="CELLRANGE">
+                    <a:fld id="{B53A2CC1-14A1-483A-9003-FC99FD497E97}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2914,7 +2956,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F291855D-887A-4EDE-98F8-CBB3BF439A92}" type="CELLRANGE">
+                    <a:fld id="{184D8317-CBB3-4122-BA50-E5DC0295AF4F}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2954,7 +2996,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{511C5DFF-2CBC-48EC-82B5-2C8B66B75EA9}" type="CELLRANGE">
+                    <a:fld id="{0F68361A-93D9-422C-9AB5-DB1B3BD3FEC7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2987,7 +3029,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2491E26B-A6F5-433C-AB92-5DCCA14D38A6}" type="CELLRANGE">
+                    <a:fld id="{3BF57178-6D44-4452-BAF1-2F4785F324F7}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3021,7 +3063,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E9CD9CE5-0D65-47BE-9F72-4181162DFE37}" type="CELLRANGE">
+                    <a:fld id="{F783E00E-5E12-41F2-8E59-C5862ED67C20}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3055,7 +3097,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CAF197C4-92E5-49ED-8F01-DF658FF57ADC}" type="CELLRANGE">
+                    <a:fld id="{57ACCFC7-C475-49BF-BDE0-85A607588428}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3095,7 +3137,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{13188D13-156F-41F7-B272-F79475D2C849}" type="CELLRANGE">
+                    <a:fld id="{172CE78F-3C5C-4405-8D12-775657AB3020}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3128,7 +3170,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AA784A6F-7FE1-4E85-8224-129EF2E8193B}" type="CELLRANGE">
+                    <a:fld id="{03172627-9DAD-4A2B-B5D3-A18A41CDFF4E}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3162,7 +3204,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F79C917C-BF3C-49B9-831F-D68710DA67AB}" type="CELLRANGE">
+                    <a:fld id="{E618B08E-8D89-4F3A-A863-BD9F0ED94CDC}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3196,7 +3238,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{33B22198-DC2E-4751-8BD9-28CDBD09FEA1}" type="CELLRANGE">
+                    <a:fld id="{3220B4F6-AF77-4C0A-A337-295C57D8EDA3}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3483,7 +3525,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7C56593B-4B78-4F80-8A32-48DBA6A4EDA0}" type="CELLRANGE">
+                    <a:fld id="{FC6F262E-D39A-42D0-B77A-228BAAC2F909}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3835,7 +3877,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{96663825-D926-4187-9D5C-FF262E630F68}" type="CELLRANGE">
+                    <a:fld id="{6A5A758C-4A2E-4B31-8FE1-C2D6D6551344}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4592,7 +4634,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{939E9027-1DF3-4020-B585-326F6F921A21}" type="CELLRANGE">
+                    <a:fld id="{48EE5BEE-8961-4B8F-8938-742EBB24002F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4831,7 +4873,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CDAAD3BE-39FF-47DD-B847-4458EA561BA2}" type="CELLRANGE">
+                    <a:fld id="{210A4633-8FCD-41D2-9FE8-0BFBE1A5F493}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4870,7 +4912,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B61300D7-E9C4-4BC7-B2C4-896755110296}" type="CELLRANGE">
+                    <a:fld id="{C667309A-C37B-4BDD-AFE2-F92B72F8D959}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4909,7 +4951,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3BD97821-5D06-44D1-8B7D-05DCCA76374A}" type="CELLRANGE">
+                    <a:fld id="{3DE6C866-7853-4C90-BAC0-9B9E8D3A8DC6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4948,7 +4990,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{467C1288-BCDC-4341-B159-37D64B0FD294}" type="CELLRANGE">
+                    <a:fld id="{8F7F7699-CD0D-4D30-85F7-E507D1425650}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4987,7 +5029,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{12B5A670-914A-4F61-AF35-BC513C4D6A0C}" type="CELLRANGE">
+                    <a:fld id="{829A5CC0-09B9-4ACB-B7F0-6A14DD3E22E9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5026,7 +5068,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E7F99F28-0868-4FB1-86A8-B2D76F206218}" type="CELLRANGE">
+                    <a:fld id="{FE539BCF-38C0-4C53-815D-9FE5B1ACD912}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5065,7 +5107,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8EAE693F-7D1B-4584-8F74-67FFF8C23DE6}" type="CELLRANGE">
+                    <a:fld id="{E901A443-45E4-4734-AA48-9E0B2E4E4CAE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5104,7 +5146,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4F4D5CD7-408C-40CF-8DC5-F3179D723CB3}" type="CELLRANGE">
+                    <a:fld id="{8CC9B019-2276-4B9C-BC8B-B9573FAE89B7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5137,7 +5179,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{543752ED-831D-4850-ABC2-FC9838B54BF7}" type="CELLRANGE">
+                    <a:fld id="{669E3963-B308-48FA-BE12-314805F60E03}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5177,7 +5219,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8A04F2AE-4488-4E54-A09B-176EA5135C49}" type="CELLRANGE">
+                    <a:fld id="{003C152F-2818-4538-ACB3-2E109836C1FA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5430,7 +5472,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AF42EA38-C8BA-4D64-AE0B-6F63377120CC}" type="CELLRANGE">
+                    <a:fld id="{DFC56CD2-9284-44BB-B928-B8C264D3E512}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5602,7 +5644,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E4290617-4956-4FAD-A0D5-03C75EA1BD5A}" type="CELLRANGE">
+                    <a:fld id="{7EEA224E-DBC3-4914-9107-36CB19B82486}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5778,7 +5820,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9175B15D-F156-4C69-97A3-1D33C7A2A98A}" type="CELLRANGE">
+                    <a:fld id="{E39AFAC4-B799-4DE7-9B72-B62E3AAD2ACF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5954,7 +5996,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3E26DECF-604A-4733-8B9F-EC316F516166}" type="CELLRANGE">
+                    <a:fld id="{313337D1-0342-45A7-9377-B19DFDAE8D7F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10923,10 +10965,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EED96773-F711-4C89-AB88-84FFC233CDF5}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10936,9 +10978,10 @@
     <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>93</v>
       </c>
@@ -10954,8 +10997,11 @@
       <c r="E1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>104</v>
       </c>
@@ -10971,8 +11017,11 @@
       <c r="E2">
         <v>1.498</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>105</v>
       </c>
@@ -10988,8 +11037,11 @@
       <c r="E3">
         <v>0.99399999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>106</v>
       </c>
@@ -11005,8 +11057,11 @@
       <c r="E4">
         <v>1.5960000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>95</v>
       </c>
@@ -11023,7 +11078,7 @@
         <v>0.88600000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>45</v>
       </c>
@@ -11039,8 +11094,11 @@
       <c r="E6">
         <v>1.393</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>39</v>
       </c>
@@ -11056,8 +11114,11 @@
       <c r="E7">
         <v>0.78600000000000003</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>96</v>
       </c>
@@ -11073,8 +11134,11 @@
       <c r="E8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>97</v>
       </c>
@@ -11090,8 +11154,11 @@
       <c r="E9">
         <v>0.79100000000000004</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>98</v>
       </c>
@@ -11107,8 +11174,11 @@
       <c r="E10">
         <v>1.0489999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>99</v>
       </c>
@@ -11124,8 +11194,11 @@
       <c r="E11">
         <v>1.21</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
@@ -11141,8 +11214,11 @@
       <c r="E12">
         <v>1.3260000000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>100</v>
       </c>
@@ -11158,8 +11234,11 @@
       <c r="E13">
         <v>0.78900000000000003</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>107</v>
       </c>
@@ -11172,13 +11251,16 @@
       <c r="D14">
         <v>189</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>37</v>
       </c>

</xml_diff>